<commit_message>
Use google sheet instead excel
</commit_message>
<xml_diff>
--- a/public/datas/gems.xlsx
+++ b/public/datas/gems.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Lnnnnn\My projects\pop-convenience-web-app\public\datas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC5F3A73-8978-4A1F-AD6C-2D47DD372686}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BE42DCE-40A9-4206-AEF7-64BCD2063A06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10245" yWindow="0" windowWidth="10245" windowHeight="10920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="5 star" sheetId="1" r:id="rId1"/>
@@ -151,7 +151,7 @@
   <numFmts count="1">
     <numFmt numFmtId="187" formatCode="[$฿-41E]#,##0.00"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -175,6 +175,13 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial Unicode MS"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
@@ -215,7 +222,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -245,6 +252,8 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -465,9 +474,9 @@
   </sheetPr>
   <dimension ref="A1:M51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F31" sqref="F31"/>
+      <selection pane="bottomLeft" activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
@@ -1475,9 +1484,9 @@
   </sheetPr>
   <dimension ref="A1:M51"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G29" sqref="G29"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G41" sqref="G41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
@@ -1547,17 +1556,17 @@
       <c r="D3" s="2">
         <v>340</v>
       </c>
-      <c r="E3" s="7">
-        <v>340</v>
-      </c>
-      <c r="F3" s="7">
-        <v>340</v>
-      </c>
-      <c r="G3" s="7">
-        <v>340</v>
-      </c>
-      <c r="H3" s="7">
-        <v>340</v>
+      <c r="E3" s="18">
+        <v>445</v>
+      </c>
+      <c r="F3" s="18">
+        <v>445</v>
+      </c>
+      <c r="G3" s="18">
+        <v>445</v>
+      </c>
+      <c r="H3" s="18">
+        <v>445</v>
       </c>
     </row>
     <row r="4" spans="1:13">
@@ -1573,17 +1582,17 @@
       <c r="D4" s="2">
         <v>555</v>
       </c>
-      <c r="E4" s="7">
-        <v>555</v>
-      </c>
-      <c r="F4" s="7">
-        <v>555</v>
-      </c>
-      <c r="G4" s="7">
-        <v>555</v>
-      </c>
-      <c r="H4" s="7">
-        <v>555</v>
+      <c r="E4" s="18">
+        <v>740</v>
+      </c>
+      <c r="F4" s="18">
+        <v>740</v>
+      </c>
+      <c r="G4" s="18">
+        <v>740</v>
+      </c>
+      <c r="H4" s="18">
+        <v>740</v>
       </c>
     </row>
     <row r="5" spans="1:13">
@@ -1599,17 +1608,17 @@
       <c r="D5" s="2">
         <v>800</v>
       </c>
-      <c r="E5" s="7">
-        <v>800</v>
-      </c>
-      <c r="F5" s="7">
-        <v>800</v>
-      </c>
-      <c r="G5" s="7">
-        <v>800</v>
-      </c>
-      <c r="H5" s="7">
-        <v>800</v>
+      <c r="E5" s="18">
+        <v>1065</v>
+      </c>
+      <c r="F5" s="18">
+        <v>1065</v>
+      </c>
+      <c r="G5" s="18">
+        <v>1065</v>
+      </c>
+      <c r="H5" s="18">
+        <v>1065</v>
       </c>
     </row>
     <row r="6" spans="1:13">
@@ -1639,7 +1648,7 @@
       </c>
       <c r="K6" s="8">
         <f>SUM(E2:E21)</f>
-        <v>93865</v>
+        <v>94420</v>
       </c>
     </row>
     <row r="7" spans="1:13">
@@ -1725,11 +1734,11 @@
       </c>
       <c r="K9" s="8">
         <f>SUM(E2:E10)</f>
-        <v>13400</v>
+        <v>13955</v>
       </c>
       <c r="M9" s="8">
         <f>K9+K10</f>
-        <v>82465</v>
+        <v>83020</v>
       </c>
     </row>
     <row r="10" spans="1:13">
@@ -1795,7 +1804,7 @@
       </c>
       <c r="K11" s="8">
         <f>SUM(E2:E20)</f>
-        <v>82465</v>
+        <v>83020</v>
       </c>
     </row>
     <row r="12" spans="1:13">
@@ -3261,10 +3270,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:L1000"/>
+  <dimension ref="A1:L999"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:H14"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
@@ -3351,11 +3360,11 @@
         <v>3750</v>
       </c>
       <c r="G3" s="1">
-        <f t="shared" ref="G2:G14" si="2">C3/F3</f>
+        <f t="shared" ref="G3:G21" si="2">C3/F3</f>
         <v>132.53333333333333</v>
       </c>
       <c r="H3">
-        <f t="shared" ref="H3:H14" si="3">F3/C3</f>
+        <f t="shared" ref="H3:H21" si="3">F3/C3</f>
         <v>7.545271629778672E-3</v>
       </c>
     </row>
@@ -3693,62 +3702,181 @@
       </c>
     </row>
     <row r="15" spans="1:12">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
+      <c r="A15" s="2">
+        <v>53636631</v>
+      </c>
+      <c r="B15" s="2">
+        <v>53253631</v>
+      </c>
+      <c r="C15" s="2">
+        <f>A15-B15</f>
+        <v>383000</v>
+      </c>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
+      <c r="F15" s="2">
+        <v>2450</v>
+      </c>
+      <c r="G15" s="1">
+        <f t="shared" si="2"/>
+        <v>156.32653061224491</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="3"/>
+        <v>6.3968668407310709E-3</v>
+      </c>
     </row>
     <row r="16" spans="1:12">
-      <c r="A16" s="2"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
+      <c r="A16" s="2">
+        <v>53253631</v>
+      </c>
+      <c r="B16" s="2">
+        <v>52861631</v>
+      </c>
+      <c r="C16" s="2">
+        <f>A16-B16</f>
+        <v>392000</v>
+      </c>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-    </row>
-    <row r="17" spans="1:6">
-      <c r="A17" s="2"/>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
+      <c r="F16" s="2">
+        <v>2850</v>
+      </c>
+      <c r="G16" s="17">
+        <f t="shared" si="2"/>
+        <v>137.54385964912279</v>
+      </c>
+      <c r="H16">
+        <f t="shared" si="3"/>
+        <v>7.2704081632653057E-3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" s="2">
+        <v>52861631</v>
+      </c>
+      <c r="B17" s="2">
+        <v>45184631</v>
+      </c>
+      <c r="C17" s="2">
+        <f>A17-B17</f>
+        <v>7677000</v>
+      </c>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-    </row>
-    <row r="18" spans="1:6">
-      <c r="A18" s="2"/>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
+      <c r="F17" s="2">
+        <v>55900</v>
+      </c>
+      <c r="G17" s="17">
+        <f t="shared" si="2"/>
+        <v>137.3345259391771</v>
+      </c>
+      <c r="H17">
+        <f t="shared" si="3"/>
+        <v>7.281490165429204E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" s="2">
+        <v>44035631</v>
+      </c>
+      <c r="B18" s="2">
+        <v>43282631</v>
+      </c>
+      <c r="C18" s="2">
+        <f>A18-B18</f>
+        <v>753000</v>
+      </c>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-    </row>
-    <row r="19" spans="1:6">
-      <c r="A19" s="2"/>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
+      <c r="F18" s="2">
+        <v>5300</v>
+      </c>
+      <c r="G18" s="17">
+        <f t="shared" si="2"/>
+        <v>142.0754716981132</v>
+      </c>
+      <c r="H18">
+        <f t="shared" si="3"/>
+        <v>7.0385126162018589E-3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" s="2">
+        <v>43282631</v>
+      </c>
+      <c r="B19" s="2">
+        <v>42525631</v>
+      </c>
+      <c r="C19" s="2">
+        <f>A19-B19</f>
+        <v>757000</v>
+      </c>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-    </row>
-    <row r="20" spans="1:6">
-      <c r="A20" s="2"/>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
+      <c r="F19" s="2">
+        <v>5650</v>
+      </c>
+      <c r="G19" s="17">
+        <f t="shared" si="2"/>
+        <v>133.98230088495575</v>
+      </c>
+      <c r="H19">
+        <f t="shared" si="3"/>
+        <v>7.4636723910171728E-3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" s="2">
+        <v>42525631</v>
+      </c>
+      <c r="B20" s="2">
+        <v>41787631</v>
+      </c>
+      <c r="C20" s="2">
+        <f>A20-B20</f>
+        <v>738000</v>
+      </c>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-    </row>
-    <row r="21" spans="1:6">
-      <c r="A21" s="2"/>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
+      <c r="F20" s="2">
+        <v>5650</v>
+      </c>
+      <c r="G20" s="17">
+        <f t="shared" si="2"/>
+        <v>130.61946902654867</v>
+      </c>
+      <c r="H20">
+        <f t="shared" si="3"/>
+        <v>7.6558265582655823E-3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21" s="2">
+        <v>41787631</v>
+      </c>
+      <c r="B21" s="2">
+        <v>38051631</v>
+      </c>
+      <c r="C21" s="2">
+        <f>A21-B21</f>
+        <v>3736000</v>
+      </c>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-    </row>
-    <row r="22" spans="1:6">
+      <c r="F21" s="2">
+        <v>25900</v>
+      </c>
+      <c r="G21" s="17">
+        <f t="shared" si="2"/>
+        <v>144.24710424710426</v>
+      </c>
+      <c r="H21">
+        <f t="shared" si="3"/>
+        <v>6.9325481798715206E-3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
@@ -3756,7 +3884,7 @@
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:8">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
@@ -3764,7 +3892,7 @@
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:8">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
@@ -3772,7 +3900,7 @@
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:8">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
@@ -3780,7 +3908,7 @@
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:8">
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
@@ -3788,7 +3916,7 @@
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:8">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
@@ -3796,7 +3924,7 @@
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:8">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
@@ -3804,7 +3932,7 @@
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:8">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
@@ -3812,7 +3940,7 @@
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:8">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
@@ -3820,7 +3948,7 @@
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:8">
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
@@ -3828,7 +3956,7 @@
       <c r="E31" s="2"/>
       <c r="F31" s="2"/>
     </row>
-    <row r="32" spans="1:6">
+    <row r="32" spans="1:8">
       <c r="A32" s="2"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
@@ -11571,14 +11699,6 @@
       <c r="D999" s="2"/>
       <c r="E999" s="2"/>
       <c r="F999" s="2"/>
-    </row>
-    <row r="1000" spans="1:6">
-      <c r="A1000" s="2"/>
-      <c r="B1000" s="2"/>
-      <c r="C1000" s="2"/>
-      <c r="D1000" s="2"/>
-      <c r="E1000" s="2"/>
-      <c r="F1000" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -11589,7 +11709,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{479D1952-7C35-45DF-BE56-1E39F9D31BAB}">
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -11618,7 +11738,7 @@
       </c>
       <c r="B2" s="13">
         <f>AVERAGE(pricing!G1:INDEX(pricing!G:G, COUNTA(pricing!G:G)))</f>
-        <v>140.44804238983991</v>
+        <v>140.39769065625927</v>
       </c>
       <c r="C2" s="9" t="s">
         <v>18</v>
@@ -11661,7 +11781,7 @@
       </c>
       <c r="B5" s="15">
         <f>AVERAGE(pricing!H1:INDEX(pricing!H:H, COUNT(pricing!H:H)))</f>
-        <v>7.1723364627473349E-3</v>
+        <v>7.160601103772782E-3</v>
       </c>
       <c r="C5" s="9" t="s">
         <v>18</v>

</xml_diff>